<commit_message>
Working on how to index
</commit_message>
<xml_diff>
--- a/AlternativeLinearInterpolation.xlsx
+++ b/AlternativeLinearInterpolation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:11_{EC8882F0-A692-4D10-A122-C2641FAA17F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63FF1CD-4C5A-47E5-8A1A-8D685089D565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -19,11 +19,14 @@
   </sheets>
   <definedNames>
     <definedName name="_nData">Report!$E$7:$E$18</definedName>
+    <definedName name="_nmax">Report!$I$6</definedName>
+    <definedName name="_nmin">Report!$I$5</definedName>
+    <definedName name="_nx">Report!$I$7</definedName>
     <definedName name="HD_Date">_xlfn.LET(_xlpm.dt, TODAY(),      _xlpm.y,  YEAR(_xlpm.dt),      _xlpm.m,  MONTH(_xlpm.dt),      _xlpm.d,  DAY(_xlpm.dt),      TEXT(DATE(_xlpm.y,_xlpm.m,_xlpm.d),"dd-mmm-yyyy")     )</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="7" r:id="rId4"/>
+    <pivotCache cacheId="8" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -65,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="27">
   <si>
     <t>FROM:</t>
   </si>
@@ -128,6 +131,24 @@
   </si>
   <si>
     <t>Metadata Tabs</t>
+  </si>
+  <si>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>Down</t>
+  </si>
+  <si>
+    <t>In</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>var</t>
   </si>
 </sst>
 </file>
@@ -312,7 +333,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -322,7 +343,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -908,7 +928,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -1200,15 +1220,15 @@
   <sheetPr codeName="Sheet1">
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:I18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1217,69 +1237,114 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>20-Aug-2024</v>
+        <v>21-Aug-2024</v>
       </c>
       <c r="C3" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5">
+        <f>MIN(_nData)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>25</v>
+      </c>
+      <c r="I6">
+        <f>MAX(E7:E17)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>26</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>21</v>
+      </c>
+      <c r="I8" t="b">
+        <f>IF(_nx&gt;_nmax,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>22</v>
+      </c>
+      <c r="I9" t="b">
+        <f>_nx&lt;_nmin</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" t="b">
+        <f>IF(MEDIAN(_nmin,_nmax,_nx)=_nx,TRUE,FALSE)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E11">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E12">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E13">
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E14">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E15">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="E16">
         <v>10</v>
       </c>
@@ -1337,7 +1402,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>20-Aug-2024</v>
+        <v>21-Aug-2024</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -1473,19 +1538,15 @@
       <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20">
         <v>1</v>
       </c>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9">
+      <c r="F20">
         <v>1</v>
       </c>
     </row>
@@ -1493,11 +1554,10 @@
       <c r="C21">
         <v>2</v>
       </c>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9">
+      <c r="E21">
         <v>2</v>
       </c>
-      <c r="F21" s="9">
+      <c r="F21">
         <v>2</v>
       </c>
     </row>
@@ -1505,19 +1565,15 @@
       <c r="B22" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="9"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="D23" s="9">
+      <c r="D23">
         <v>3</v>
       </c>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9">
+      <c r="F23">
         <v>3</v>
       </c>
     </row>
@@ -1525,11 +1581,10 @@
       <c r="C24">
         <v>2</v>
       </c>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9">
+      <c r="E24">
         <v>4</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24">
         <v>4</v>
       </c>
     </row>
@@ -1537,19 +1592,15 @@
       <c r="B25" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26">
         <v>5</v>
       </c>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9">
+      <c r="F26">
         <v>5</v>
       </c>
     </row>
@@ -1557,11 +1608,10 @@
       <c r="C27">
         <v>2</v>
       </c>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9">
+      <c r="E27">
         <v>6</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27">
         <v>6</v>
       </c>
     </row>
@@ -1569,13 +1619,13 @@
       <c r="B28" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28">
         <v>9</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28">
         <v>12</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28">
         <v>21</v>
       </c>
     </row>
@@ -1648,7 +1698,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>20-Aug-2024</v>
+        <v>21-Aug-2024</v>
       </c>
       <c r="C3" s="2"/>
     </row>

</xml_diff>

<commit_message>
Playing with my early test code
</commit_message>
<xml_diff>
--- a/AlternativeLinearInterpolation.xlsx
+++ b/AlternativeLinearInterpolation.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28015"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E605CBB-1677-45D7-A4AD-EA6BED159BFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F93BDDC9-1270-499B-8BC4-0488FD15F158}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -26,7 +26,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="8" r:id="rId4"/>
+    <pivotCache cacheId="1" r:id="rId4"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -1181,445 +1181,445 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="147"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.99999999999999911</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.3000000000000003</c:v>
+                  <c:v>1.7000000000000002</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.5999999999999996</c:v>
+                  <c:v>2.3999999999999986</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.9000000000000004</c:v>
+                  <c:v>3.0999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.1999999999999993</c:v>
+                  <c:v>3.7999999999999989</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.5</c:v>
+                  <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.8000000000000007</c:v>
+                  <c:v>5.2000000000000011</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.0999999999999996</c:v>
+                  <c:v>5.8999999999999986</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.4000000000000004</c:v>
+                  <c:v>6.6</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3.6999999999999993</c:v>
+                  <c:v>7.2999999999999989</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.5</c:v>
+                  <c:v>9.9000000000000057</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.0000000000000018</c:v>
+                  <c:v>11.800000000000004</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.5</c:v>
+                  <c:v>13.699999999999996</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6</c:v>
+                  <c:v>15.600000000000001</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6.5</c:v>
+                  <c:v>17.5</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.0000000000000018</c:v>
+                  <c:v>19.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.5000000000000018</c:v>
+                  <c:v>21.300000000000011</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>8</c:v>
+                  <c:v>23.200000000000003</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>8.5</c:v>
+                  <c:v>25.1</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>9</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9.6999999999999993</c:v>
+                  <c:v>30.700000000000003</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>10.400000000000002</c:v>
+                  <c:v>34.400000000000006</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>11.099999999999998</c:v>
+                  <c:v>38.099999999999994</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>11.799999999999997</c:v>
+                  <c:v>41.8</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>12.5</c:v>
+                  <c:v>45.5</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>13.2</c:v>
+                  <c:v>49.200000000000017</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>13.900000000000002</c:v>
+                  <c:v>52.900000000000006</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>14.599999999999998</c:v>
+                  <c:v>56.599999999999994</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>15.3</c:v>
+                  <c:v>60.299999999999983</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>16</c:v>
+                  <c:v>63.999999999999972</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>16.899999999999999</c:v>
+                  <c:v>70.099999999999937</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>17.800000000000004</c:v>
+                  <c:v>76.199999999999989</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>18.699999999999996</c:v>
+                  <c:v>82.299999999999955</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>19.600000000000001</c:v>
+                  <c:v>88.399999999999977</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>20.5</c:v>
+                  <c:v>94.5</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>21.4</c:v>
+                  <c:v>100.59999999999997</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>22.300000000000004</c:v>
+                  <c:v>106.69999999999999</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>23.199999999999996</c:v>
+                  <c:v>112.79999999999995</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>24.1</c:v>
+                  <c:v>118.89999999999998</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>25</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>26.099999999999994</c:v>
+                  <c:v>134.09999999999997</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>27.200000000000003</c:v>
+                  <c:v>143.19999999999999</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>28.299999999999997</c:v>
+                  <c:v>152.30000000000001</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>29.4</c:v>
+                  <c:v>161.40000000000003</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>30.5</c:v>
+                  <c:v>170.5</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>31.599999999999994</c:v>
+                  <c:v>179.59999999999997</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>32.699999999999996</c:v>
+                  <c:v>188.70000000000005</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>33.799999999999997</c:v>
+                  <c:v>197.79999999999995</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>34.9</c:v>
+                  <c:v>206.89999999999998</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>36</c:v>
+                  <c:v>216</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>37.299999999999997</c:v>
+                  <c:v>228.69999999999993</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>38.600000000000009</c:v>
+                  <c:v>241.39999999999998</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>39.899999999999991</c:v>
+                  <c:v>254.09999999999991</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>41.2</c:v>
+                  <c:v>266.80000000000007</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>42.500000000000128</c:v>
+                  <c:v>279.50000000000125</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>43.8</c:v>
+                  <c:v>292.19999999999993</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>45.100000000000009</c:v>
+                  <c:v>304.89999999999998</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>46.400000000000119</c:v>
+                  <c:v>317.60000000000116</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>47.700000000000131</c:v>
+                  <c:v>330.30000000000132</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>49.000000000000142</c:v>
+                  <c:v>343.00000000000159</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>50.499999999999986</c:v>
+                  <c:v>359.89999999999986</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>52.000000000000142</c:v>
+                  <c:v>376.80000000000177</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>53.500000000000142</c:v>
+                  <c:v>393.70000000000164</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>55.000000000000142</c:v>
+                  <c:v>410.60000000000173</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>56.500000000000142</c:v>
+                  <c:v>427.50000000000159</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>58.000000000000156</c:v>
+                  <c:v>444.40000000000168</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>59.500000000000142</c:v>
+                  <c:v>461.30000000000177</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>61.000000000000142</c:v>
+                  <c:v>478.20000000000164</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>62.500000000000156</c:v>
+                  <c:v>495.10000000000173</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>64.000000000000171</c:v>
+                  <c:v>512.00000000000227</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>65.700000000000188</c:v>
+                  <c:v>533.70000000000232</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>67.400000000000176</c:v>
+                  <c:v>555.40000000000214</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>69.100000000000165</c:v>
+                  <c:v>577.10000000000218</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>70.800000000000153</c:v>
+                  <c:v>598.800000000002</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>72.500000000000171</c:v>
+                  <c:v>620.50000000000227</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>74.200000000000188</c:v>
+                  <c:v>642.20000000000232</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>75.900000000000176</c:v>
+                  <c:v>663.90000000000214</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>77.600000000000165</c:v>
+                  <c:v>685.60000000000218</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>79.300000000000153</c:v>
+                  <c:v>707.300000000002</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>81.000000000000199</c:v>
+                  <c:v>729.00000000000273</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>82.900000000000205</c:v>
+                  <c:v>756.10000000000264</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>84.80000000000021</c:v>
+                  <c:v>783.20000000000255</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>86.700000000000188</c:v>
+                  <c:v>810.30000000000246</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>88.600000000000193</c:v>
+                  <c:v>837.40000000000236</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>90.500000000000227</c:v>
+                  <c:v>864.50000000000273</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>92.400000000000205</c:v>
+                  <c:v>891.60000000000264</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>94.30000000000021</c:v>
+                  <c:v>918.70000000000255</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>96.200000000000188</c:v>
+                  <c:v>945.80000000000246</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>98.100000000000193</c:v>
+                  <c:v>972.90000000000236</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>100</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>102.1</c:v>
+                  <c:v>1033.0999999999999</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>104.19999999999999</c:v>
+                  <c:v>1066.1999999999998</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>106.30000000000001</c:v>
+                  <c:v>1099.3000000000002</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>108.4</c:v>
+                  <c:v>1132.4000000000001</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>110.5</c:v>
+                  <c:v>1165.5</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>112.6</c:v>
+                  <c:v>1198.5999999999999</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>114.69999999999999</c:v>
+                  <c:v>1231.6999999999998</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>116.80000000000001</c:v>
+                  <c:v>1264.8000000000002</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>118.9</c:v>
+                  <c:v>1297.9000000000001</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>120.99999999999997</c:v>
+                  <c:v>1331</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>123.29999999999998</c:v>
+                  <c:v>1370.6999999999998</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>125.59999999999997</c:v>
+                  <c:v>1410.3999999999996</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>127.89999999999998</c:v>
+                  <c:v>1450.1000000000004</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>130.19999999999999</c:v>
+                  <c:v>1489.8000000000002</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>132.5</c:v>
+                  <c:v>1529.5</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>134.79999999999995</c:v>
+                  <c:v>1569.1999999999998</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>137.09999999999997</c:v>
+                  <c:v>1608.8999999999996</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>139.39999999999998</c:v>
+                  <c:v>1648.6000000000004</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>141.69999999999999</c:v>
+                  <c:v>1688.3000000000002</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>144</c:v>
+                  <c:v>1728</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>146.29999999999995</c:v>
+                  <c:v>1767.6999999999998</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>148.59999999999997</c:v>
+                  <c:v>1807.3999999999996</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>150.89999999999998</c:v>
+                  <c:v>1847.1000000000004</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>153.19999999999999</c:v>
+                  <c:v>1886.8000000000002</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>155.5</c:v>
+                  <c:v>1926.5</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>157.79999999999995</c:v>
+                  <c:v>1966.1999999999998</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>160.09999999999997</c:v>
+                  <c:v>2005.8999999999996</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>162.39999999999998</c:v>
+                  <c:v>2045.6000000000004</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>164.7</c:v>
+                  <c:v>2085.3000000000002</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>167</c:v>
+                  <c:v>2125</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>169.29999999999995</c:v>
+                  <c:v>2164.6999999999998</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>171.59999999999997</c:v>
+                  <c:v>2204.3999999999996</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>173.90000000000003</c:v>
+                  <c:v>2244.1000000000004</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>176.2</c:v>
+                  <c:v>2283.8000000000002</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>178.5</c:v>
+                  <c:v>2323.5</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>180.8</c:v>
+                  <c:v>2363.1999999999998</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>183.09999999999997</c:v>
+                  <c:v>2402.8999999999996</c:v>
                 </c:pt>
                 <c:pt idx="128">
-                  <c:v>185.40000000000003</c:v>
+                  <c:v>2442.6000000000004</c:v>
                 </c:pt>
                 <c:pt idx="129">
-                  <c:v>187.7</c:v>
+                  <c:v>2482.3000000000002</c:v>
                 </c:pt>
                 <c:pt idx="130">
-                  <c:v>190</c:v>
+                  <c:v>2522</c:v>
                 </c:pt>
                 <c:pt idx="131">
-                  <c:v>192.3</c:v>
+                  <c:v>2561.6999999999998</c:v>
                 </c:pt>
                 <c:pt idx="132">
-                  <c:v>194.59999999999997</c:v>
+                  <c:v>2601.3999999999996</c:v>
                 </c:pt>
                 <c:pt idx="133">
-                  <c:v>196.90000000000003</c:v>
+                  <c:v>2641.1000000000004</c:v>
                 </c:pt>
                 <c:pt idx="134">
-                  <c:v>199.2</c:v>
+                  <c:v>2680.8</c:v>
                 </c:pt>
                 <c:pt idx="135">
-                  <c:v>201.5</c:v>
+                  <c:v>2720.5</c:v>
                 </c:pt>
                 <c:pt idx="136">
-                  <c:v>203.8</c:v>
+                  <c:v>2760.2</c:v>
                 </c:pt>
                 <c:pt idx="137">
-                  <c:v>206.09999999999997</c:v>
+                  <c:v>2799.8999999999996</c:v>
                 </c:pt>
                 <c:pt idx="138">
-                  <c:v>208.40000000000003</c:v>
+                  <c:v>2839.6000000000004</c:v>
                 </c:pt>
                 <c:pt idx="139">
-                  <c:v>210.7</c:v>
+                  <c:v>2879.3</c:v>
                 </c:pt>
                 <c:pt idx="140">
-                  <c:v>213</c:v>
+                  <c:v>2919</c:v>
                 </c:pt>
                 <c:pt idx="141">
-                  <c:v>215.3</c:v>
+                  <c:v>2958.7</c:v>
                 </c:pt>
                 <c:pt idx="142">
-                  <c:v>217.59999999999997</c:v>
+                  <c:v>2998.3999999999996</c:v>
                 </c:pt>
                 <c:pt idx="143">
-                  <c:v>219.90000000000003</c:v>
+                  <c:v>3038.1000000000004</c:v>
                 </c:pt>
                 <c:pt idx="144">
-                  <c:v>222.2</c:v>
+                  <c:v>3077.8</c:v>
                 </c:pt>
                 <c:pt idx="145">
-                  <c:v>224.5</c:v>
+                  <c:v>3117.5</c:v>
                 </c:pt>
                 <c:pt idx="146">
-                  <c:v>226.8</c:v>
+                  <c:v>3157.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1711,37 +1711,37 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>9</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>25</c:v>
+                  <c:v>125</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>36</c:v>
+                  <c:v>216</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>49</c:v>
+                  <c:v>343</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>64</c:v>
+                  <c:v>512</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>81</c:v>
+                  <c:v>729</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>100</c:v>
+                  <c:v>1000</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>121</c:v>
+                  <c:v>1331</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>144</c:v>
+                  <c:v>1728</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1768,6 +1768,7 @@
         <c:axId val="2122342575"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="-10"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1830,6 +1831,7 @@
         <c:axId val="2122341135"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="-100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2609,8 +2611,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="3166111" y="262835"/>
-          <a:ext cx="2200275" cy="455350"/>
+          <a:off x="3158491" y="270455"/>
+          <a:ext cx="2205990" cy="464875"/>
           <a:chOff x="3162301" y="274265"/>
           <a:chExt cx="2198370" cy="459814"/>
         </a:xfrm>
@@ -2829,7 +2831,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{F44C8824-5739-49B7-BCFF-9C42983375DF}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B17:F28" firstHeaderRow="1" firstDataRow="2" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" compact="0" showAll="0" defaultSubtotal="0">
@@ -3123,8 +3125,8 @@
   </sheetPr>
   <dimension ref="A1:L229"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3151,7 +3153,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>21-Aug-2024</v>
+        <v>22-Aug-2024</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -3178,14 +3180,14 @@
         <v>1</v>
       </c>
       <c r="F7">
-        <f>E7^2</f>
+        <f>E7^3</f>
         <v>1</v>
       </c>
       <c r="H7" t="s">
         <v>26</v>
       </c>
       <c r="I7" s="10">
-        <v>20</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -3193,19 +3195,19 @@
         <v>2</v>
       </c>
       <c r="F8">
-        <f t="shared" ref="F8:F18" si="0">E8^2</f>
-        <v>4</v>
+        <f t="shared" ref="F8:F18" si="0">E8^3</f>
+        <v>8</v>
       </c>
       <c r="H8" t="s">
         <v>21</v>
       </c>
       <c r="I8" t="b">
         <f>IF(_nx&gt;_nmax,TRUE,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" cm="1">
         <f t="array" ref="J8">TREND(F17:F18,E17:E18,_nx)</f>
-        <v>328</v>
+        <v>-7006</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3214,18 +3216,18 @@
       </c>
       <c r="F9">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="H9" t="s">
         <v>22</v>
       </c>
       <c r="I9" t="b">
         <f>_nx&lt;_nmin</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" cm="1">
         <f t="array" ref="J9">TREND(F7:F8,E7:E8,_nx)</f>
-        <v>58</v>
+        <v>-76.000000000000014</v>
       </c>
       <c r="K9" s="11"/>
       <c r="L9" s="11"/>
@@ -3236,7 +3238,7 @@
       </c>
       <c r="F10">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>64</v>
       </c>
       <c r="H10" t="s">
         <v>23</v>
@@ -3245,16 +3247,16 @@
         <f>IF(MEDIAN(_nmin,_nmax,_nx)=_nx,TRUE,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="9" t="e">
         <f>_xlfn.XMATCH(_nx,_nData,-1)</f>
-        <v>12</v>
-      </c>
-      <c r="K10" s="10" cm="1">
+        <v>#N/A</v>
+      </c>
+      <c r="K10" s="10" t="e" cm="1">
         <f t="array" ref="K10:L10">J10+{0,1}</f>
-        <v>12</v>
-      </c>
-      <c r="L10" s="10">
-        <v>13</v>
+        <v>#N/A</v>
+      </c>
+      <c r="L10" s="10" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -3263,18 +3265,18 @@
       </c>
       <c r="F11">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>125</v>
       </c>
       <c r="J11" t="s">
         <v>27</v>
       </c>
-      <c r="K11" cm="1">
+      <c r="K11" t="e" cm="1">
         <f t="array" ref="K11">INDEX(_nData,K10)</f>
-        <v>12</v>
+        <v>#N/A</v>
       </c>
       <c r="L11" t="e" cm="1">
         <f t="array" ref="L11">INDEX(_nData,L10)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -3283,18 +3285,18 @@
       </c>
       <c r="F12">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>216</v>
       </c>
       <c r="J12" t="s">
         <v>28</v>
       </c>
-      <c r="K12" cm="1">
+      <c r="K12" t="e" cm="1">
         <f t="array" ref="K12">INDEX($F$7:$F$18,K10)</f>
-        <v>144</v>
+        <v>#N/A</v>
       </c>
       <c r="L12" t="e" cm="1">
         <f t="array" ref="L12">INDEX($F$7:$F$18,L10)</f>
-        <v>#REF!</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -3303,7 +3305,7 @@
       </c>
       <c r="F13">
         <f t="shared" si="0"/>
-        <v>49</v>
+        <v>343</v>
       </c>
       <c r="K13" t="e" cm="1">
         <f t="array" ref="K13">TREND(K12:L12,K11:L11,_nx)</f>
@@ -3316,11 +3318,11 @@
       </c>
       <c r="F14">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>512</v>
       </c>
       <c r="I14" cm="1">
         <f t="array" ref="I14">_xlfn.SWITCH(TRUE,I8,J8,I9,J9,K13)</f>
-        <v>328</v>
+        <v>-76.000000000000014</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -3329,7 +3331,7 @@
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>81</v>
+        <v>729</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -3338,7 +3340,7 @@
       </c>
       <c r="F16">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="17" spans="5:11" x14ac:dyDescent="0.25">
@@ -3347,7 +3349,7 @@
       </c>
       <c r="F17">
         <f t="shared" si="0"/>
-        <v>121</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="18" spans="5:11" x14ac:dyDescent="0.25">
@@ -3356,11 +3358,11 @@
       </c>
       <c r="F18">
         <f t="shared" si="0"/>
-        <v>144</v>
+        <v>1728</v>
       </c>
       <c r="K18">
         <f>I14</f>
-        <v>328</v>
+        <v>-76.000000000000014</v>
       </c>
     </row>
     <row r="19" spans="5:11" x14ac:dyDescent="0.25">
@@ -3369,7 +3371,7 @@
       </c>
       <c r="K19">
         <f t="dataTable" ref="K19:K229" dt2D="0" dtr="0" r1="I7"/>
-        <v>1</v>
+        <v>0.99999999999999911</v>
       </c>
     </row>
     <row r="20" spans="5:11" x14ac:dyDescent="0.25">
@@ -3377,7 +3379,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="K20">
-        <v>1.3000000000000003</v>
+        <v>1.7000000000000002</v>
       </c>
     </row>
     <row r="21" spans="5:11" x14ac:dyDescent="0.25">
@@ -3385,7 +3387,7 @@
         <v>1.2</v>
       </c>
       <c r="K21">
-        <v>1.5999999999999996</v>
+        <v>2.3999999999999986</v>
       </c>
     </row>
     <row r="22" spans="5:11" x14ac:dyDescent="0.25">
@@ -3393,7 +3395,7 @@
         <v>1.3</v>
       </c>
       <c r="K22">
-        <v>1.9000000000000004</v>
+        <v>3.0999999999999996</v>
       </c>
     </row>
     <row r="23" spans="5:11" x14ac:dyDescent="0.25">
@@ -3401,7 +3403,7 @@
         <v>1.4</v>
       </c>
       <c r="K23">
-        <v>2.1999999999999993</v>
+        <v>3.7999999999999989</v>
       </c>
     </row>
     <row r="24" spans="5:11" x14ac:dyDescent="0.25">
@@ -3409,7 +3411,7 @@
         <v>1.5</v>
       </c>
       <c r="K24">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
     </row>
     <row r="25" spans="5:11" x14ac:dyDescent="0.25">
@@ -3417,7 +3419,7 @@
         <v>1.6</v>
       </c>
       <c r="K25">
-        <v>2.8000000000000007</v>
+        <v>5.2000000000000011</v>
       </c>
     </row>
     <row r="26" spans="5:11" x14ac:dyDescent="0.25">
@@ -3425,7 +3427,7 @@
         <v>1.7</v>
       </c>
       <c r="K26">
-        <v>3.0999999999999996</v>
+        <v>5.8999999999999986</v>
       </c>
     </row>
     <row r="27" spans="5:11" x14ac:dyDescent="0.25">
@@ -3433,7 +3435,7 @@
         <v>1.8</v>
       </c>
       <c r="K27">
-        <v>3.4000000000000004</v>
+        <v>6.6</v>
       </c>
     </row>
     <row r="28" spans="5:11" x14ac:dyDescent="0.25">
@@ -3441,7 +3443,7 @@
         <v>1.9</v>
       </c>
       <c r="K28">
-        <v>3.6999999999999993</v>
+        <v>7.2999999999999989</v>
       </c>
     </row>
     <row r="29" spans="5:11" x14ac:dyDescent="0.25">
@@ -3449,7 +3451,7 @@
         <v>2</v>
       </c>
       <c r="K29">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="5:11" x14ac:dyDescent="0.25">
@@ -3457,7 +3459,7 @@
         <v>2.1</v>
       </c>
       <c r="K30">
-        <v>4.5</v>
+        <v>9.9000000000000057</v>
       </c>
     </row>
     <row r="31" spans="5:11" x14ac:dyDescent="0.25">
@@ -3465,7 +3467,7 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="K31">
-        <v>5.0000000000000018</v>
+        <v>11.800000000000004</v>
       </c>
     </row>
     <row r="32" spans="5:11" x14ac:dyDescent="0.25">
@@ -3473,7 +3475,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="K32">
-        <v>5.5</v>
+        <v>13.699999999999996</v>
       </c>
     </row>
     <row r="33" spans="10:11" x14ac:dyDescent="0.25">
@@ -3481,7 +3483,7 @@
         <v>2.4</v>
       </c>
       <c r="K33">
-        <v>6</v>
+        <v>15.600000000000001</v>
       </c>
     </row>
     <row r="34" spans="10:11" x14ac:dyDescent="0.25">
@@ -3489,7 +3491,7 @@
         <v>2.5</v>
       </c>
       <c r="K34">
-        <v>6.5</v>
+        <v>17.5</v>
       </c>
     </row>
     <row r="35" spans="10:11" x14ac:dyDescent="0.25">
@@ -3497,7 +3499,7 @@
         <v>2.6</v>
       </c>
       <c r="K35">
-        <v>7.0000000000000018</v>
+        <v>19.400000000000006</v>
       </c>
     </row>
     <row r="36" spans="10:11" x14ac:dyDescent="0.25">
@@ -3505,7 +3507,7 @@
         <v>2.7</v>
       </c>
       <c r="K36">
-        <v>7.5000000000000018</v>
+        <v>21.300000000000011</v>
       </c>
     </row>
     <row r="37" spans="10:11" x14ac:dyDescent="0.25">
@@ -3513,7 +3515,7 @@
         <v>2.8</v>
       </c>
       <c r="K37">
-        <v>8</v>
+        <v>23.200000000000003</v>
       </c>
     </row>
     <row r="38" spans="10:11" x14ac:dyDescent="0.25">
@@ -3521,7 +3523,7 @@
         <v>2.9</v>
       </c>
       <c r="K38">
-        <v>8.5</v>
+        <v>25.1</v>
       </c>
     </row>
     <row r="39" spans="10:11" x14ac:dyDescent="0.25">
@@ -3529,7 +3531,7 @@
         <v>3</v>
       </c>
       <c r="K39">
-        <v>9</v>
+        <v>27</v>
       </c>
     </row>
     <row r="40" spans="10:11" x14ac:dyDescent="0.25">
@@ -3537,7 +3539,7 @@
         <v>3.1</v>
       </c>
       <c r="K40">
-        <v>9.6999999999999993</v>
+        <v>30.700000000000003</v>
       </c>
     </row>
     <row r="41" spans="10:11" x14ac:dyDescent="0.25">
@@ -3545,7 +3547,7 @@
         <v>3.2</v>
       </c>
       <c r="K41">
-        <v>10.400000000000002</v>
+        <v>34.400000000000006</v>
       </c>
     </row>
     <row r="42" spans="10:11" x14ac:dyDescent="0.25">
@@ -3553,7 +3555,7 @@
         <v>3.3</v>
       </c>
       <c r="K42">
-        <v>11.099999999999998</v>
+        <v>38.099999999999994</v>
       </c>
     </row>
     <row r="43" spans="10:11" x14ac:dyDescent="0.25">
@@ -3561,7 +3563,7 @@
         <v>3.4</v>
       </c>
       <c r="K43">
-        <v>11.799999999999997</v>
+        <v>41.8</v>
       </c>
     </row>
     <row r="44" spans="10:11" x14ac:dyDescent="0.25">
@@ -3569,7 +3571,7 @@
         <v>3.5</v>
       </c>
       <c r="K44">
-        <v>12.5</v>
+        <v>45.5</v>
       </c>
     </row>
     <row r="45" spans="10:11" x14ac:dyDescent="0.25">
@@ -3577,7 +3579,7 @@
         <v>3.6</v>
       </c>
       <c r="K45">
-        <v>13.2</v>
+        <v>49.200000000000017</v>
       </c>
     </row>
     <row r="46" spans="10:11" x14ac:dyDescent="0.25">
@@ -3585,7 +3587,7 @@
         <v>3.7</v>
       </c>
       <c r="K46">
-        <v>13.900000000000002</v>
+        <v>52.900000000000006</v>
       </c>
     </row>
     <row r="47" spans="10:11" x14ac:dyDescent="0.25">
@@ -3593,7 +3595,7 @@
         <v>3.8</v>
       </c>
       <c r="K47">
-        <v>14.599999999999998</v>
+        <v>56.599999999999994</v>
       </c>
     </row>
     <row r="48" spans="10:11" x14ac:dyDescent="0.25">
@@ -3601,7 +3603,7 @@
         <v>3.9</v>
       </c>
       <c r="K48">
-        <v>15.3</v>
+        <v>60.299999999999983</v>
       </c>
     </row>
     <row r="49" spans="10:11" x14ac:dyDescent="0.25">
@@ -3609,7 +3611,7 @@
         <v>4</v>
       </c>
       <c r="K49">
-        <v>16</v>
+        <v>63.999999999999972</v>
       </c>
     </row>
     <row r="50" spans="10:11" x14ac:dyDescent="0.25">
@@ -3617,7 +3619,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="K50">
-        <v>16.899999999999999</v>
+        <v>70.099999999999937</v>
       </c>
     </row>
     <row r="51" spans="10:11" x14ac:dyDescent="0.25">
@@ -3625,7 +3627,7 @@
         <v>4.2</v>
       </c>
       <c r="K51">
-        <v>17.800000000000004</v>
+        <v>76.199999999999989</v>
       </c>
     </row>
     <row r="52" spans="10:11" x14ac:dyDescent="0.25">
@@ -3633,7 +3635,7 @@
         <v>4.3</v>
       </c>
       <c r="K52">
-        <v>18.699999999999996</v>
+        <v>82.299999999999955</v>
       </c>
     </row>
     <row r="53" spans="10:11" x14ac:dyDescent="0.25">
@@ -3641,7 +3643,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="K53">
-        <v>19.600000000000001</v>
+        <v>88.399999999999977</v>
       </c>
     </row>
     <row r="54" spans="10:11" x14ac:dyDescent="0.25">
@@ -3649,7 +3651,7 @@
         <v>4.5</v>
       </c>
       <c r="K54">
-        <v>20.5</v>
+        <v>94.5</v>
       </c>
     </row>
     <row r="55" spans="10:11" x14ac:dyDescent="0.25">
@@ -3657,7 +3659,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="K55">
-        <v>21.4</v>
+        <v>100.59999999999997</v>
       </c>
     </row>
     <row r="56" spans="10:11" x14ac:dyDescent="0.25">
@@ -3665,7 +3667,7 @@
         <v>4.7</v>
       </c>
       <c r="K56">
-        <v>22.300000000000004</v>
+        <v>106.69999999999999</v>
       </c>
     </row>
     <row r="57" spans="10:11" x14ac:dyDescent="0.25">
@@ -3673,7 +3675,7 @@
         <v>4.8</v>
       </c>
       <c r="K57">
-        <v>23.199999999999996</v>
+        <v>112.79999999999995</v>
       </c>
     </row>
     <row r="58" spans="10:11" x14ac:dyDescent="0.25">
@@ -3681,7 +3683,7 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="K58">
-        <v>24.1</v>
+        <v>118.89999999999998</v>
       </c>
     </row>
     <row r="59" spans="10:11" x14ac:dyDescent="0.25">
@@ -3689,7 +3691,7 @@
         <v>5</v>
       </c>
       <c r="K59">
-        <v>25</v>
+        <v>125</v>
       </c>
     </row>
     <row r="60" spans="10:11" x14ac:dyDescent="0.25">
@@ -3697,7 +3699,7 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="K60">
-        <v>26.099999999999994</v>
+        <v>134.09999999999997</v>
       </c>
     </row>
     <row r="61" spans="10:11" x14ac:dyDescent="0.25">
@@ -3705,7 +3707,7 @@
         <v>5.2</v>
       </c>
       <c r="K61">
-        <v>27.200000000000003</v>
+        <v>143.19999999999999</v>
       </c>
     </row>
     <row r="62" spans="10:11" x14ac:dyDescent="0.25">
@@ -3713,7 +3715,7 @@
         <v>5.3</v>
       </c>
       <c r="K62">
-        <v>28.299999999999997</v>
+        <v>152.30000000000001</v>
       </c>
     </row>
     <row r="63" spans="10:11" x14ac:dyDescent="0.25">
@@ -3721,7 +3723,7 @@
         <v>5.4</v>
       </c>
       <c r="K63">
-        <v>29.4</v>
+        <v>161.40000000000003</v>
       </c>
     </row>
     <row r="64" spans="10:11" x14ac:dyDescent="0.25">
@@ -3729,7 +3731,7 @@
         <v>5.5</v>
       </c>
       <c r="K64">
-        <v>30.5</v>
+        <v>170.5</v>
       </c>
     </row>
     <row r="65" spans="10:11" x14ac:dyDescent="0.25">
@@ -3737,7 +3739,7 @@
         <v>5.6</v>
       </c>
       <c r="K65">
-        <v>31.599999999999994</v>
+        <v>179.59999999999997</v>
       </c>
     </row>
     <row r="66" spans="10:11" x14ac:dyDescent="0.25">
@@ -3745,7 +3747,7 @@
         <v>5.7</v>
       </c>
       <c r="K66">
-        <v>32.699999999999996</v>
+        <v>188.70000000000005</v>
       </c>
     </row>
     <row r="67" spans="10:11" x14ac:dyDescent="0.25">
@@ -3753,7 +3755,7 @@
         <v>5.8</v>
       </c>
       <c r="K67">
-        <v>33.799999999999997</v>
+        <v>197.79999999999995</v>
       </c>
     </row>
     <row r="68" spans="10:11" x14ac:dyDescent="0.25">
@@ -3761,7 +3763,7 @@
         <v>5.9</v>
       </c>
       <c r="K68">
-        <v>34.9</v>
+        <v>206.89999999999998</v>
       </c>
     </row>
     <row r="69" spans="10:11" x14ac:dyDescent="0.25">
@@ -3769,7 +3771,7 @@
         <v>6</v>
       </c>
       <c r="K69">
-        <v>36</v>
+        <v>216</v>
       </c>
     </row>
     <row r="70" spans="10:11" x14ac:dyDescent="0.25">
@@ -3777,7 +3779,7 @@
         <v>6.1</v>
       </c>
       <c r="K70">
-        <v>37.299999999999997</v>
+        <v>228.69999999999993</v>
       </c>
     </row>
     <row r="71" spans="10:11" x14ac:dyDescent="0.25">
@@ -3785,7 +3787,7 @@
         <v>6.2</v>
       </c>
       <c r="K71">
-        <v>38.600000000000009</v>
+        <v>241.39999999999998</v>
       </c>
     </row>
     <row r="72" spans="10:11" x14ac:dyDescent="0.25">
@@ -3793,7 +3795,7 @@
         <v>6.3</v>
       </c>
       <c r="K72">
-        <v>39.899999999999991</v>
+        <v>254.09999999999991</v>
       </c>
     </row>
     <row r="73" spans="10:11" x14ac:dyDescent="0.25">
@@ -3801,7 +3803,7 @@
         <v>6.4</v>
       </c>
       <c r="K73">
-        <v>41.2</v>
+        <v>266.80000000000007</v>
       </c>
     </row>
     <row r="74" spans="10:11" x14ac:dyDescent="0.25">
@@ -3809,7 +3811,7 @@
         <v>6.5000000000000098</v>
       </c>
       <c r="K74">
-        <v>42.500000000000128</v>
+        <v>279.50000000000125</v>
       </c>
     </row>
     <row r="75" spans="10:11" x14ac:dyDescent="0.25">
@@ -3817,7 +3819,7 @@
         <v>6.6</v>
       </c>
       <c r="K75">
-        <v>43.8</v>
+        <v>292.19999999999993</v>
       </c>
     </row>
     <row r="76" spans="10:11" x14ac:dyDescent="0.25">
@@ -3825,7 +3827,7 @@
         <v>6.7</v>
       </c>
       <c r="K76">
-        <v>45.100000000000009</v>
+        <v>304.89999999999998</v>
       </c>
     </row>
     <row r="77" spans="10:11" x14ac:dyDescent="0.25">
@@ -3833,7 +3835,7 @@
         <v>6.8000000000000096</v>
       </c>
       <c r="K77">
-        <v>46.400000000000119</v>
+        <v>317.60000000000116</v>
       </c>
     </row>
     <row r="78" spans="10:11" x14ac:dyDescent="0.25">
@@ -3841,7 +3843,7 @@
         <v>6.9000000000000101</v>
       </c>
       <c r="K78">
-        <v>47.700000000000131</v>
+        <v>330.30000000000132</v>
       </c>
     </row>
     <row r="79" spans="10:11" x14ac:dyDescent="0.25">
@@ -3849,7 +3851,7 @@
         <v>7.0000000000000098</v>
       </c>
       <c r="K79">
-        <v>49.000000000000142</v>
+        <v>343.00000000000159</v>
       </c>
     </row>
     <row r="80" spans="10:11" x14ac:dyDescent="0.25">
@@ -3857,7 +3859,7 @@
         <v>7.1</v>
       </c>
       <c r="K80">
-        <v>50.499999999999986</v>
+        <v>359.89999999999986</v>
       </c>
     </row>
     <row r="81" spans="10:11" x14ac:dyDescent="0.25">
@@ -3865,7 +3867,7 @@
         <v>7.2000000000000099</v>
       </c>
       <c r="K81">
-        <v>52.000000000000142</v>
+        <v>376.80000000000177</v>
       </c>
     </row>
     <row r="82" spans="10:11" x14ac:dyDescent="0.25">
@@ -3873,7 +3875,7 @@
         <v>7.3000000000000096</v>
       </c>
       <c r="K82">
-        <v>53.500000000000142</v>
+        <v>393.70000000000164</v>
       </c>
     </row>
     <row r="83" spans="10:11" x14ac:dyDescent="0.25">
@@ -3881,7 +3883,7 @@
         <v>7.4000000000000101</v>
       </c>
       <c r="K83">
-        <v>55.000000000000142</v>
+        <v>410.60000000000173</v>
       </c>
     </row>
     <row r="84" spans="10:11" x14ac:dyDescent="0.25">
@@ -3889,7 +3891,7 @@
         <v>7.5000000000000098</v>
       </c>
       <c r="K84">
-        <v>56.500000000000142</v>
+        <v>427.50000000000159</v>
       </c>
     </row>
     <row r="85" spans="10:11" x14ac:dyDescent="0.25">
@@ -3897,7 +3899,7 @@
         <v>7.6000000000000103</v>
       </c>
       <c r="K85">
-        <v>58.000000000000156</v>
+        <v>444.40000000000168</v>
       </c>
     </row>
     <row r="86" spans="10:11" x14ac:dyDescent="0.25">
@@ -3905,7 +3907,7 @@
         <v>7.7000000000000099</v>
       </c>
       <c r="K86">
-        <v>59.500000000000142</v>
+        <v>461.30000000000177</v>
       </c>
     </row>
     <row r="87" spans="10:11" x14ac:dyDescent="0.25">
@@ -3913,7 +3915,7 @@
         <v>7.8000000000000096</v>
       </c>
       <c r="K87">
-        <v>61.000000000000142</v>
+        <v>478.20000000000164</v>
       </c>
     </row>
     <row r="88" spans="10:11" x14ac:dyDescent="0.25">
@@ -3921,7 +3923,7 @@
         <v>7.9000000000000101</v>
       </c>
       <c r="K88">
-        <v>62.500000000000156</v>
+        <v>495.10000000000173</v>
       </c>
     </row>
     <row r="89" spans="10:11" x14ac:dyDescent="0.25">
@@ -3929,7 +3931,7 @@
         <v>8.0000000000000107</v>
       </c>
       <c r="K89">
-        <v>64.000000000000171</v>
+        <v>512.00000000000227</v>
       </c>
     </row>
     <row r="90" spans="10:11" x14ac:dyDescent="0.25">
@@ -3937,7 +3939,7 @@
         <v>8.1000000000000103</v>
       </c>
       <c r="K90">
-        <v>65.700000000000188</v>
+        <v>533.70000000000232</v>
       </c>
     </row>
     <row r="91" spans="10:11" x14ac:dyDescent="0.25">
@@ -3945,7 +3947,7 @@
         <v>8.2000000000000099</v>
       </c>
       <c r="K91">
-        <v>67.400000000000176</v>
+        <v>555.40000000000214</v>
       </c>
     </row>
     <row r="92" spans="10:11" x14ac:dyDescent="0.25">
@@ -3953,7 +3955,7 @@
         <v>8.3000000000000096</v>
       </c>
       <c r="K92">
-        <v>69.100000000000165</v>
+        <v>577.10000000000218</v>
       </c>
     </row>
     <row r="93" spans="10:11" x14ac:dyDescent="0.25">
@@ -3961,7 +3963,7 @@
         <v>8.4000000000000092</v>
       </c>
       <c r="K93">
-        <v>70.800000000000153</v>
+        <v>598.800000000002</v>
       </c>
     </row>
     <row r="94" spans="10:11" x14ac:dyDescent="0.25">
@@ -3969,7 +3971,7 @@
         <v>8.5000000000000107</v>
       </c>
       <c r="K94">
-        <v>72.500000000000171</v>
+        <v>620.50000000000227</v>
       </c>
     </row>
     <row r="95" spans="10:11" x14ac:dyDescent="0.25">
@@ -3977,7 +3979,7 @@
         <v>8.6000000000000103</v>
       </c>
       <c r="K95">
-        <v>74.200000000000188</v>
+        <v>642.20000000000232</v>
       </c>
     </row>
     <row r="96" spans="10:11" x14ac:dyDescent="0.25">
@@ -3985,7 +3987,7 @@
         <v>8.7000000000000099</v>
       </c>
       <c r="K96">
-        <v>75.900000000000176</v>
+        <v>663.90000000000214</v>
       </c>
     </row>
     <row r="97" spans="10:11" x14ac:dyDescent="0.25">
@@ -3993,7 +3995,7 @@
         <v>8.8000000000000096</v>
       </c>
       <c r="K97">
-        <v>77.600000000000165</v>
+        <v>685.60000000000218</v>
       </c>
     </row>
     <row r="98" spans="10:11" x14ac:dyDescent="0.25">
@@ -4001,7 +4003,7 @@
         <v>8.9000000000000092</v>
       </c>
       <c r="K98">
-        <v>79.300000000000153</v>
+        <v>707.300000000002</v>
       </c>
     </row>
     <row r="99" spans="10:11" x14ac:dyDescent="0.25">
@@ -4009,7 +4011,7 @@
         <v>9.0000000000000107</v>
       </c>
       <c r="K99">
-        <v>81.000000000000199</v>
+        <v>729.00000000000273</v>
       </c>
     </row>
     <row r="100" spans="10:11" x14ac:dyDescent="0.25">
@@ -4017,7 +4019,7 @@
         <v>9.1000000000000103</v>
       </c>
       <c r="K100">
-        <v>82.900000000000205</v>
+        <v>756.10000000000264</v>
       </c>
     </row>
     <row r="101" spans="10:11" x14ac:dyDescent="0.25">
@@ -4025,7 +4027,7 @@
         <v>9.2000000000000099</v>
       </c>
       <c r="K101">
-        <v>84.80000000000021</v>
+        <v>783.20000000000255</v>
       </c>
     </row>
     <row r="102" spans="10:11" x14ac:dyDescent="0.25">
@@ -4033,7 +4035,7 @@
         <v>9.3000000000000096</v>
       </c>
       <c r="K102">
-        <v>86.700000000000188</v>
+        <v>810.30000000000246</v>
       </c>
     </row>
     <row r="103" spans="10:11" x14ac:dyDescent="0.25">
@@ -4041,7 +4043,7 @@
         <v>9.4000000000000092</v>
       </c>
       <c r="K103">
-        <v>88.600000000000193</v>
+        <v>837.40000000000236</v>
       </c>
     </row>
     <row r="104" spans="10:11" x14ac:dyDescent="0.25">
@@ -4049,7 +4051,7 @@
         <v>9.5000000000000107</v>
       </c>
       <c r="K104">
-        <v>90.500000000000227</v>
+        <v>864.50000000000273</v>
       </c>
     </row>
     <row r="105" spans="10:11" x14ac:dyDescent="0.25">
@@ -4057,7 +4059,7 @@
         <v>9.6000000000000103</v>
       </c>
       <c r="K105">
-        <v>92.400000000000205</v>
+        <v>891.60000000000264</v>
       </c>
     </row>
     <row r="106" spans="10:11" x14ac:dyDescent="0.25">
@@ -4065,7 +4067,7 @@
         <v>9.7000000000000099</v>
       </c>
       <c r="K106">
-        <v>94.30000000000021</v>
+        <v>918.70000000000255</v>
       </c>
     </row>
     <row r="107" spans="10:11" x14ac:dyDescent="0.25">
@@ -4073,7 +4075,7 @@
         <v>9.8000000000000096</v>
       </c>
       <c r="K107">
-        <v>96.200000000000188</v>
+        <v>945.80000000000246</v>
       </c>
     </row>
     <row r="108" spans="10:11" x14ac:dyDescent="0.25">
@@ -4081,7 +4083,7 @@
         <v>9.9000000000000092</v>
       </c>
       <c r="K108">
-        <v>98.100000000000193</v>
+        <v>972.90000000000236</v>
       </c>
     </row>
     <row r="109" spans="10:11" x14ac:dyDescent="0.25">
@@ -4089,7 +4091,7 @@
         <v>10</v>
       </c>
       <c r="K109">
-        <v>100</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="110" spans="10:11" x14ac:dyDescent="0.25">
@@ -4097,7 +4099,7 @@
         <v>10.1</v>
       </c>
       <c r="K110">
-        <v>102.1</v>
+        <v>1033.0999999999999</v>
       </c>
     </row>
     <row r="111" spans="10:11" x14ac:dyDescent="0.25">
@@ -4105,7 +4107,7 @@
         <v>10.199999999999999</v>
       </c>
       <c r="K111">
-        <v>104.19999999999999</v>
+        <v>1066.1999999999998</v>
       </c>
     </row>
     <row r="112" spans="10:11" x14ac:dyDescent="0.25">
@@ -4113,7 +4115,7 @@
         <v>10.3</v>
       </c>
       <c r="K112">
-        <v>106.30000000000001</v>
+        <v>1099.3000000000002</v>
       </c>
     </row>
     <row r="113" spans="10:11" x14ac:dyDescent="0.25">
@@ -4121,7 +4123,7 @@
         <v>10.4</v>
       </c>
       <c r="K113">
-        <v>108.4</v>
+        <v>1132.4000000000001</v>
       </c>
     </row>
     <row r="114" spans="10:11" x14ac:dyDescent="0.25">
@@ -4129,7 +4131,7 @@
         <v>10.5</v>
       </c>
       <c r="K114">
-        <v>110.5</v>
+        <v>1165.5</v>
       </c>
     </row>
     <row r="115" spans="10:11" x14ac:dyDescent="0.25">
@@ -4137,7 +4139,7 @@
         <v>10.6</v>
       </c>
       <c r="K115">
-        <v>112.6</v>
+        <v>1198.5999999999999</v>
       </c>
     </row>
     <row r="116" spans="10:11" x14ac:dyDescent="0.25">
@@ -4145,7 +4147,7 @@
         <v>10.7</v>
       </c>
       <c r="K116">
-        <v>114.69999999999999</v>
+        <v>1231.6999999999998</v>
       </c>
     </row>
     <row r="117" spans="10:11" x14ac:dyDescent="0.25">
@@ -4153,7 +4155,7 @@
         <v>10.8</v>
       </c>
       <c r="K117">
-        <v>116.80000000000001</v>
+        <v>1264.8000000000002</v>
       </c>
     </row>
     <row r="118" spans="10:11" x14ac:dyDescent="0.25">
@@ -4161,7 +4163,7 @@
         <v>10.9</v>
       </c>
       <c r="K118">
-        <v>118.9</v>
+        <v>1297.9000000000001</v>
       </c>
     </row>
     <row r="119" spans="10:11" x14ac:dyDescent="0.25">
@@ -4169,7 +4171,7 @@
         <v>11</v>
       </c>
       <c r="K119">
-        <v>120.99999999999997</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="120" spans="10:11" x14ac:dyDescent="0.25">
@@ -4177,7 +4179,7 @@
         <v>11.1</v>
       </c>
       <c r="K120">
-        <v>123.29999999999998</v>
+        <v>1370.6999999999998</v>
       </c>
     </row>
     <row r="121" spans="10:11" x14ac:dyDescent="0.25">
@@ -4185,7 +4187,7 @@
         <v>11.2</v>
       </c>
       <c r="K121">
-        <v>125.59999999999997</v>
+        <v>1410.3999999999996</v>
       </c>
     </row>
     <row r="122" spans="10:11" x14ac:dyDescent="0.25">
@@ -4193,7 +4195,7 @@
         <v>11.3</v>
       </c>
       <c r="K122">
-        <v>127.89999999999998</v>
+        <v>1450.1000000000004</v>
       </c>
     </row>
     <row r="123" spans="10:11" x14ac:dyDescent="0.25">
@@ -4201,7 +4203,7 @@
         <v>11.4</v>
       </c>
       <c r="K123">
-        <v>130.19999999999999</v>
+        <v>1489.8000000000002</v>
       </c>
     </row>
     <row r="124" spans="10:11" x14ac:dyDescent="0.25">
@@ -4209,7 +4211,7 @@
         <v>11.5</v>
       </c>
       <c r="K124">
-        <v>132.5</v>
+        <v>1529.5</v>
       </c>
     </row>
     <row r="125" spans="10:11" x14ac:dyDescent="0.25">
@@ -4217,7 +4219,7 @@
         <v>11.6</v>
       </c>
       <c r="K125">
-        <v>134.79999999999995</v>
+        <v>1569.1999999999998</v>
       </c>
     </row>
     <row r="126" spans="10:11" x14ac:dyDescent="0.25">
@@ -4225,7 +4227,7 @@
         <v>11.7</v>
       </c>
       <c r="K126">
-        <v>137.09999999999997</v>
+        <v>1608.8999999999996</v>
       </c>
     </row>
     <row r="127" spans="10:11" x14ac:dyDescent="0.25">
@@ -4233,7 +4235,7 @@
         <v>11.8</v>
       </c>
       <c r="K127">
-        <v>139.39999999999998</v>
+        <v>1648.6000000000004</v>
       </c>
     </row>
     <row r="128" spans="10:11" x14ac:dyDescent="0.25">
@@ -4241,7 +4243,7 @@
         <v>11.9</v>
       </c>
       <c r="K128">
-        <v>141.69999999999999</v>
+        <v>1688.3000000000002</v>
       </c>
     </row>
     <row r="129" spans="10:11" x14ac:dyDescent="0.25">
@@ -4249,7 +4251,7 @@
         <v>12</v>
       </c>
       <c r="K129">
-        <v>144</v>
+        <v>1728</v>
       </c>
     </row>
     <row r="130" spans="10:11" x14ac:dyDescent="0.25">
@@ -4257,7 +4259,7 @@
         <v>12.1</v>
       </c>
       <c r="K130">
-        <v>146.29999999999995</v>
+        <v>1767.6999999999998</v>
       </c>
     </row>
     <row r="131" spans="10:11" x14ac:dyDescent="0.25">
@@ -4265,7 +4267,7 @@
         <v>12.2</v>
       </c>
       <c r="K131">
-        <v>148.59999999999997</v>
+        <v>1807.3999999999996</v>
       </c>
     </row>
     <row r="132" spans="10:11" x14ac:dyDescent="0.25">
@@ -4273,7 +4275,7 @@
         <v>12.3</v>
       </c>
       <c r="K132">
-        <v>150.89999999999998</v>
+        <v>1847.1000000000004</v>
       </c>
     </row>
     <row r="133" spans="10:11" x14ac:dyDescent="0.25">
@@ -4281,7 +4283,7 @@
         <v>12.4</v>
       </c>
       <c r="K133">
-        <v>153.19999999999999</v>
+        <v>1886.8000000000002</v>
       </c>
     </row>
     <row r="134" spans="10:11" x14ac:dyDescent="0.25">
@@ -4289,7 +4291,7 @@
         <v>12.5</v>
       </c>
       <c r="K134">
-        <v>155.5</v>
+        <v>1926.5</v>
       </c>
     </row>
     <row r="135" spans="10:11" x14ac:dyDescent="0.25">
@@ -4297,7 +4299,7 @@
         <v>12.6</v>
       </c>
       <c r="K135">
-        <v>157.79999999999995</v>
+        <v>1966.1999999999998</v>
       </c>
     </row>
     <row r="136" spans="10:11" x14ac:dyDescent="0.25">
@@ -4305,7 +4307,7 @@
         <v>12.7</v>
       </c>
       <c r="K136">
-        <v>160.09999999999997</v>
+        <v>2005.8999999999996</v>
       </c>
     </row>
     <row r="137" spans="10:11" x14ac:dyDescent="0.25">
@@ -4313,7 +4315,7 @@
         <v>12.8</v>
       </c>
       <c r="K137">
-        <v>162.39999999999998</v>
+        <v>2045.6000000000004</v>
       </c>
     </row>
     <row r="138" spans="10:11" x14ac:dyDescent="0.25">
@@ -4321,7 +4323,7 @@
         <v>12.9</v>
       </c>
       <c r="K138">
-        <v>164.7</v>
+        <v>2085.3000000000002</v>
       </c>
     </row>
     <row r="139" spans="10:11" x14ac:dyDescent="0.25">
@@ -4329,7 +4331,7 @@
         <v>13</v>
       </c>
       <c r="K139">
-        <v>167</v>
+        <v>2125</v>
       </c>
     </row>
     <row r="140" spans="10:11" x14ac:dyDescent="0.25">
@@ -4337,7 +4339,7 @@
         <v>13.1</v>
       </c>
       <c r="K140">
-        <v>169.29999999999995</v>
+        <v>2164.6999999999998</v>
       </c>
     </row>
     <row r="141" spans="10:11" x14ac:dyDescent="0.25">
@@ -4345,7 +4347,7 @@
         <v>13.2</v>
       </c>
       <c r="K141">
-        <v>171.59999999999997</v>
+        <v>2204.3999999999996</v>
       </c>
     </row>
     <row r="142" spans="10:11" x14ac:dyDescent="0.25">
@@ -4353,7 +4355,7 @@
         <v>13.3</v>
       </c>
       <c r="K142">
-        <v>173.90000000000003</v>
+        <v>2244.1000000000004</v>
       </c>
     </row>
     <row r="143" spans="10:11" x14ac:dyDescent="0.25">
@@ -4361,7 +4363,7 @@
         <v>13.4</v>
       </c>
       <c r="K143">
-        <v>176.2</v>
+        <v>2283.8000000000002</v>
       </c>
     </row>
     <row r="144" spans="10:11" x14ac:dyDescent="0.25">
@@ -4369,7 +4371,7 @@
         <v>13.5</v>
       </c>
       <c r="K144">
-        <v>178.5</v>
+        <v>2323.5</v>
       </c>
     </row>
     <row r="145" spans="10:11" x14ac:dyDescent="0.25">
@@ -4377,7 +4379,7 @@
         <v>13.6</v>
       </c>
       <c r="K145">
-        <v>180.8</v>
+        <v>2363.1999999999998</v>
       </c>
     </row>
     <row r="146" spans="10:11" x14ac:dyDescent="0.25">
@@ -4385,7 +4387,7 @@
         <v>13.7</v>
       </c>
       <c r="K146">
-        <v>183.09999999999997</v>
+        <v>2402.8999999999996</v>
       </c>
     </row>
     <row r="147" spans="10:11" x14ac:dyDescent="0.25">
@@ -4393,7 +4395,7 @@
         <v>13.8</v>
       </c>
       <c r="K147">
-        <v>185.40000000000003</v>
+        <v>2442.6000000000004</v>
       </c>
     </row>
     <row r="148" spans="10:11" x14ac:dyDescent="0.25">
@@ -4401,7 +4403,7 @@
         <v>13.9</v>
       </c>
       <c r="K148">
-        <v>187.7</v>
+        <v>2482.3000000000002</v>
       </c>
     </row>
     <row r="149" spans="10:11" x14ac:dyDescent="0.25">
@@ -4409,7 +4411,7 @@
         <v>14</v>
       </c>
       <c r="K149">
-        <v>190</v>
+        <v>2522</v>
       </c>
     </row>
     <row r="150" spans="10:11" x14ac:dyDescent="0.25">
@@ -4417,7 +4419,7 @@
         <v>14.1</v>
       </c>
       <c r="K150">
-        <v>192.3</v>
+        <v>2561.6999999999998</v>
       </c>
     </row>
     <row r="151" spans="10:11" x14ac:dyDescent="0.25">
@@ -4425,7 +4427,7 @@
         <v>14.2</v>
       </c>
       <c r="K151">
-        <v>194.59999999999997</v>
+        <v>2601.3999999999996</v>
       </c>
     </row>
     <row r="152" spans="10:11" x14ac:dyDescent="0.25">
@@ -4433,7 +4435,7 @@
         <v>14.3</v>
       </c>
       <c r="K152">
-        <v>196.90000000000003</v>
+        <v>2641.1000000000004</v>
       </c>
     </row>
     <row r="153" spans="10:11" x14ac:dyDescent="0.25">
@@ -4441,7 +4443,7 @@
         <v>14.4</v>
       </c>
       <c r="K153">
-        <v>199.2</v>
+        <v>2680.8</v>
       </c>
     </row>
     <row r="154" spans="10:11" x14ac:dyDescent="0.25">
@@ -4449,7 +4451,7 @@
         <v>14.5</v>
       </c>
       <c r="K154">
-        <v>201.5</v>
+        <v>2720.5</v>
       </c>
     </row>
     <row r="155" spans="10:11" x14ac:dyDescent="0.25">
@@ -4457,7 +4459,7 @@
         <v>14.6</v>
       </c>
       <c r="K155">
-        <v>203.8</v>
+        <v>2760.2</v>
       </c>
     </row>
     <row r="156" spans="10:11" x14ac:dyDescent="0.25">
@@ -4465,7 +4467,7 @@
         <v>14.7</v>
       </c>
       <c r="K156">
-        <v>206.09999999999997</v>
+        <v>2799.8999999999996</v>
       </c>
     </row>
     <row r="157" spans="10:11" x14ac:dyDescent="0.25">
@@ -4473,7 +4475,7 @@
         <v>14.8</v>
       </c>
       <c r="K157">
-        <v>208.40000000000003</v>
+        <v>2839.6000000000004</v>
       </c>
     </row>
     <row r="158" spans="10:11" x14ac:dyDescent="0.25">
@@ -4481,7 +4483,7 @@
         <v>14.9</v>
       </c>
       <c r="K158">
-        <v>210.7</v>
+        <v>2879.3</v>
       </c>
     </row>
     <row r="159" spans="10:11" x14ac:dyDescent="0.25">
@@ -4489,7 +4491,7 @@
         <v>15</v>
       </c>
       <c r="K159">
-        <v>213</v>
+        <v>2919</v>
       </c>
     </row>
     <row r="160" spans="10:11" x14ac:dyDescent="0.25">
@@ -4497,7 +4499,7 @@
         <v>15.1</v>
       </c>
       <c r="K160">
-        <v>215.3</v>
+        <v>2958.7</v>
       </c>
     </row>
     <row r="161" spans="10:11" x14ac:dyDescent="0.25">
@@ -4505,7 +4507,7 @@
         <v>15.2</v>
       </c>
       <c r="K161">
-        <v>217.59999999999997</v>
+        <v>2998.3999999999996</v>
       </c>
     </row>
     <row r="162" spans="10:11" x14ac:dyDescent="0.25">
@@ -4513,7 +4515,7 @@
         <v>15.3</v>
       </c>
       <c r="K162">
-        <v>219.90000000000003</v>
+        <v>3038.1000000000004</v>
       </c>
     </row>
     <row r="163" spans="10:11" x14ac:dyDescent="0.25">
@@ -4521,7 +4523,7 @@
         <v>15.4</v>
       </c>
       <c r="K163">
-        <v>222.2</v>
+        <v>3077.8</v>
       </c>
     </row>
     <row r="164" spans="10:11" x14ac:dyDescent="0.25">
@@ -4529,7 +4531,7 @@
         <v>15.5</v>
       </c>
       <c r="K164">
-        <v>224.5</v>
+        <v>3117.5</v>
       </c>
     </row>
     <row r="165" spans="10:11" x14ac:dyDescent="0.25">
@@ -4537,7 +4539,7 @@
         <v>15.6</v>
       </c>
       <c r="K165">
-        <v>226.8</v>
+        <v>3157.2</v>
       </c>
     </row>
     <row r="166" spans="10:11" x14ac:dyDescent="0.25">
@@ -4545,7 +4547,7 @@
         <v>15.7</v>
       </c>
       <c r="K166">
-        <v>229.09999999999997</v>
+        <v>3196.8999999999996</v>
       </c>
     </row>
     <row r="167" spans="10:11" x14ac:dyDescent="0.25">
@@ -4553,7 +4555,7 @@
         <v>15.8</v>
       </c>
       <c r="K167">
-        <v>231.40000000000003</v>
+        <v>3236.6000000000004</v>
       </c>
     </row>
     <row r="168" spans="10:11" x14ac:dyDescent="0.25">
@@ -4561,7 +4563,7 @@
         <v>15.9</v>
       </c>
       <c r="K168">
-        <v>233.7</v>
+        <v>3276.3</v>
       </c>
     </row>
     <row r="169" spans="10:11" x14ac:dyDescent="0.25">
@@ -4569,7 +4571,7 @@
         <v>16</v>
       </c>
       <c r="K169">
-        <v>236</v>
+        <v>3316</v>
       </c>
     </row>
     <row r="170" spans="10:11" x14ac:dyDescent="0.25">
@@ -4577,7 +4579,7 @@
         <v>16.100000000000001</v>
       </c>
       <c r="K170">
-        <v>238.3</v>
+        <v>3355.7000000000007</v>
       </c>
     </row>
     <row r="171" spans="10:11" x14ac:dyDescent="0.25">
@@ -4585,7 +4587,7 @@
         <v>16.2</v>
       </c>
       <c r="K171">
-        <v>240.59999999999997</v>
+        <v>3395.3999999999996</v>
       </c>
     </row>
     <row r="172" spans="10:11" x14ac:dyDescent="0.25">
@@ -4593,7 +4595,7 @@
         <v>16.3</v>
       </c>
       <c r="K172">
-        <v>242.90000000000003</v>
+        <v>3435.1000000000004</v>
       </c>
     </row>
     <row r="173" spans="10:11" x14ac:dyDescent="0.25">
@@ -4601,7 +4603,7 @@
         <v>16.399999999999999</v>
       </c>
       <c r="K173">
-        <v>245.2</v>
+        <v>3474.7999999999993</v>
       </c>
     </row>
     <row r="174" spans="10:11" x14ac:dyDescent="0.25">
@@ -4609,7 +4611,7 @@
         <v>16.5</v>
       </c>
       <c r="K174">
-        <v>247.5</v>
+        <v>3514.5</v>
       </c>
     </row>
     <row r="175" spans="10:11" x14ac:dyDescent="0.25">
@@ -4617,7 +4619,7 @@
         <v>16.600000000000001</v>
       </c>
       <c r="K175">
-        <v>249.8</v>
+        <v>3554.2000000000007</v>
       </c>
     </row>
     <row r="176" spans="10:11" x14ac:dyDescent="0.25">
@@ -4625,7 +4627,7 @@
         <v>16.7</v>
       </c>
       <c r="K176">
-        <v>252.09999999999997</v>
+        <v>3593.8999999999996</v>
       </c>
     </row>
     <row r="177" spans="10:11" x14ac:dyDescent="0.25">
@@ -4633,7 +4635,7 @@
         <v>16.8</v>
       </c>
       <c r="K177">
-        <v>254.40000000000003</v>
+        <v>3633.6000000000004</v>
       </c>
     </row>
     <row r="178" spans="10:11" x14ac:dyDescent="0.25">
@@ -4641,7 +4643,7 @@
         <v>16.899999999999999</v>
       </c>
       <c r="K178">
-        <v>256.7</v>
+        <v>3673.2999999999993</v>
       </c>
     </row>
     <row r="179" spans="10:11" x14ac:dyDescent="0.25">
@@ -4649,7 +4651,7 @@
         <v>17</v>
       </c>
       <c r="K179">
-        <v>259</v>
+        <v>3713</v>
       </c>
     </row>
     <row r="180" spans="10:11" x14ac:dyDescent="0.25">
@@ -4657,7 +4659,7 @@
         <v>17.100000000000001</v>
       </c>
       <c r="K180">
-        <v>261.3</v>
+        <v>3752.7000000000007</v>
       </c>
     </row>
     <row r="181" spans="10:11" x14ac:dyDescent="0.25">
@@ -4665,7 +4667,7 @@
         <v>17.2</v>
       </c>
       <c r="K181">
-        <v>263.59999999999997</v>
+        <v>3792.3999999999996</v>
       </c>
     </row>
     <row r="182" spans="10:11" x14ac:dyDescent="0.25">
@@ -4673,7 +4675,7 @@
         <v>17.3</v>
       </c>
       <c r="K182">
-        <v>265.90000000000003</v>
+        <v>3832.1000000000004</v>
       </c>
     </row>
     <row r="183" spans="10:11" x14ac:dyDescent="0.25">
@@ -4681,7 +4683,7 @@
         <v>17.399999999999999</v>
       </c>
       <c r="K183">
-        <v>268.2</v>
+        <v>3871.7999999999993</v>
       </c>
     </row>
     <row r="184" spans="10:11" x14ac:dyDescent="0.25">
@@ -4689,7 +4691,7 @@
         <v>17.5</v>
       </c>
       <c r="K184">
-        <v>270.5</v>
+        <v>3911.5</v>
       </c>
     </row>
     <row r="185" spans="10:11" x14ac:dyDescent="0.25">
@@ -4697,7 +4699,7 @@
         <v>17.600000000000001</v>
       </c>
       <c r="K185">
-        <v>272.8</v>
+        <v>3951.2000000000007</v>
       </c>
     </row>
     <row r="186" spans="10:11" x14ac:dyDescent="0.25">
@@ -4705,7 +4707,7 @@
         <v>17.7</v>
       </c>
       <c r="K186">
-        <v>275.09999999999997</v>
+        <v>3990.8999999999996</v>
       </c>
     </row>
     <row r="187" spans="10:11" x14ac:dyDescent="0.25">
@@ -4713,7 +4715,7 @@
         <v>17.8</v>
       </c>
       <c r="K187">
-        <v>277.40000000000003</v>
+        <v>4030.6000000000004</v>
       </c>
     </row>
     <row r="188" spans="10:11" x14ac:dyDescent="0.25">
@@ -4721,7 +4723,7 @@
         <v>17.899999999999999</v>
       </c>
       <c r="K188">
-        <v>279.7</v>
+        <v>4070.2999999999993</v>
       </c>
     </row>
     <row r="189" spans="10:11" x14ac:dyDescent="0.25">
@@ -4729,7 +4731,7 @@
         <v>18</v>
       </c>
       <c r="K189">
-        <v>282</v>
+        <v>4110</v>
       </c>
     </row>
     <row r="190" spans="10:11" x14ac:dyDescent="0.25">
@@ -4737,7 +4739,7 @@
         <v>18.100000000000001</v>
       </c>
       <c r="K190">
-        <v>284.30000000000007</v>
+        <v>4149.7000000000007</v>
       </c>
     </row>
     <row r="191" spans="10:11" x14ac:dyDescent="0.25">
@@ -4745,7 +4747,7 @@
         <v>18.2</v>
       </c>
       <c r="K191">
-        <v>286.59999999999997</v>
+        <v>4189.3999999999996</v>
       </c>
     </row>
     <row r="192" spans="10:11" x14ac:dyDescent="0.25">
@@ -4753,7 +4755,7 @@
         <v>18.3</v>
       </c>
       <c r="K192">
-        <v>288.90000000000003</v>
+        <v>4229.1000000000004</v>
       </c>
     </row>
     <row r="193" spans="10:11" x14ac:dyDescent="0.25">
@@ -4761,7 +4763,7 @@
         <v>18.399999999999999</v>
       </c>
       <c r="K193">
-        <v>291.2</v>
+        <v>4268.7999999999993</v>
       </c>
     </row>
     <row r="194" spans="10:11" x14ac:dyDescent="0.25">
@@ -4769,7 +4771,7 @@
         <v>18.5</v>
       </c>
       <c r="K194">
-        <v>293.5</v>
+        <v>4308.5</v>
       </c>
     </row>
     <row r="195" spans="10:11" x14ac:dyDescent="0.25">
@@ -4777,7 +4779,7 @@
         <v>18.600000000000001</v>
       </c>
       <c r="K195">
-        <v>295.80000000000007</v>
+        <v>4348.2000000000007</v>
       </c>
     </row>
     <row r="196" spans="10:11" x14ac:dyDescent="0.25">
@@ -4785,7 +4787,7 @@
         <v>18.7</v>
       </c>
       <c r="K196">
-        <v>298.09999999999997</v>
+        <v>4387.8999999999996</v>
       </c>
     </row>
     <row r="197" spans="10:11" x14ac:dyDescent="0.25">
@@ -4793,7 +4795,7 @@
         <v>18.8</v>
       </c>
       <c r="K197">
-        <v>300.40000000000003</v>
+        <v>4427.6000000000004</v>
       </c>
     </row>
     <row r="198" spans="10:11" x14ac:dyDescent="0.25">
@@ -4801,7 +4803,7 @@
         <v>18.899999999999999</v>
       </c>
       <c r="K198">
-        <v>302.7</v>
+        <v>4467.2999999999993</v>
       </c>
     </row>
     <row r="199" spans="10:11" x14ac:dyDescent="0.25">
@@ -4809,7 +4811,7 @@
         <v>19</v>
       </c>
       <c r="K199">
-        <v>305</v>
+        <v>4507</v>
       </c>
     </row>
     <row r="200" spans="10:11" x14ac:dyDescent="0.25">
@@ -4817,7 +4819,7 @@
         <v>19.100000000000001</v>
       </c>
       <c r="K200">
-        <v>307.30000000000007</v>
+        <v>4546.7000000000007</v>
       </c>
     </row>
     <row r="201" spans="10:11" x14ac:dyDescent="0.25">
@@ -4825,7 +4827,7 @@
         <v>19.2</v>
       </c>
       <c r="K201">
-        <v>309.60000000000002</v>
+        <v>4586.3999999999996</v>
       </c>
     </row>
     <row r="202" spans="10:11" x14ac:dyDescent="0.25">
@@ -4833,7 +4835,7 @@
         <v>19.3</v>
       </c>
       <c r="K202">
-        <v>311.90000000000003</v>
+        <v>4626.1000000000004</v>
       </c>
     </row>
     <row r="203" spans="10:11" x14ac:dyDescent="0.25">
@@ -4841,7 +4843,7 @@
         <v>19.399999999999999</v>
       </c>
       <c r="K203">
-        <v>314.2</v>
+        <v>4665.7999999999993</v>
       </c>
     </row>
     <row r="204" spans="10:11" x14ac:dyDescent="0.25">
@@ -4849,7 +4851,7 @@
         <v>19.5</v>
       </c>
       <c r="K204">
-        <v>316.5</v>
+        <v>4705.5</v>
       </c>
     </row>
     <row r="205" spans="10:11" x14ac:dyDescent="0.25">
@@ -4857,7 +4859,7 @@
         <v>19.600000000000001</v>
       </c>
       <c r="K205">
-        <v>318.80000000000007</v>
+        <v>4745.2000000000007</v>
       </c>
     </row>
     <row r="206" spans="10:11" x14ac:dyDescent="0.25">
@@ -4865,7 +4867,7 @@
         <v>19.7</v>
       </c>
       <c r="K206">
-        <v>321.10000000000002</v>
+        <v>4784.8999999999996</v>
       </c>
     </row>
     <row r="207" spans="10:11" x14ac:dyDescent="0.25">
@@ -4873,7 +4875,7 @@
         <v>19.8</v>
       </c>
       <c r="K207">
-        <v>323.40000000000003</v>
+        <v>4824.6000000000004</v>
       </c>
     </row>
     <row r="208" spans="10:11" x14ac:dyDescent="0.25">
@@ -4881,7 +4883,7 @@
         <v>19.899999999999999</v>
       </c>
       <c r="K208">
-        <v>325.7</v>
+        <v>4864.2999999999993</v>
       </c>
     </row>
     <row r="209" spans="10:11" x14ac:dyDescent="0.25">
@@ -4889,7 +4891,7 @@
         <v>20</v>
       </c>
       <c r="K209">
-        <v>328</v>
+        <v>4904</v>
       </c>
     </row>
     <row r="210" spans="10:11" x14ac:dyDescent="0.25">
@@ -4897,7 +4899,7 @@
         <v>20.100000000000001</v>
       </c>
       <c r="K210">
-        <v>330.30000000000007</v>
+        <v>4943.7000000000007</v>
       </c>
     </row>
     <row r="211" spans="10:11" x14ac:dyDescent="0.25">
@@ -4905,7 +4907,7 @@
         <v>20.2</v>
       </c>
       <c r="K211">
-        <v>332.6</v>
+        <v>4983.3999999999996</v>
       </c>
     </row>
     <row r="212" spans="10:11" x14ac:dyDescent="0.25">
@@ -4913,7 +4915,7 @@
         <v>20.3</v>
       </c>
       <c r="K212">
-        <v>334.90000000000003</v>
+        <v>5023.1000000000004</v>
       </c>
     </row>
     <row r="213" spans="10:11" x14ac:dyDescent="0.25">
@@ -4921,7 +4923,7 @@
         <v>20.399999999999999</v>
       </c>
       <c r="K213">
-        <v>337.2</v>
+        <v>5062.7999999999993</v>
       </c>
     </row>
     <row r="214" spans="10:11" x14ac:dyDescent="0.25">
@@ -4929,7 +4931,7 @@
         <v>20.5</v>
       </c>
       <c r="K214">
-        <v>339.5</v>
+        <v>5102.5</v>
       </c>
     </row>
     <row r="215" spans="10:11" x14ac:dyDescent="0.25">
@@ -4937,7 +4939,7 @@
         <v>20.6</v>
       </c>
       <c r="K215">
-        <v>341.80000000000007</v>
+        <v>5142.2000000000007</v>
       </c>
     </row>
     <row r="216" spans="10:11" x14ac:dyDescent="0.25">
@@ -4945,7 +4947,7 @@
         <v>20.7</v>
       </c>
       <c r="K216">
-        <v>344.1</v>
+        <v>5181.8999999999996</v>
       </c>
     </row>
     <row r="217" spans="10:11" x14ac:dyDescent="0.25">
@@ -4953,7 +4955,7 @@
         <v>20.8</v>
       </c>
       <c r="K217">
-        <v>346.40000000000003</v>
+        <v>5221.6000000000004</v>
       </c>
     </row>
     <row r="218" spans="10:11" x14ac:dyDescent="0.25">
@@ -4961,7 +4963,7 @@
         <v>20.9</v>
       </c>
       <c r="K218">
-        <v>348.7</v>
+        <v>5261.2999999999993</v>
       </c>
     </row>
     <row r="219" spans="10:11" x14ac:dyDescent="0.25">
@@ -4969,7 +4971,7 @@
         <v>21</v>
       </c>
       <c r="K219">
-        <v>351</v>
+        <v>5301</v>
       </c>
     </row>
     <row r="220" spans="10:11" x14ac:dyDescent="0.25">
@@ -4977,7 +4979,7 @@
         <v>21.1</v>
       </c>
       <c r="K220">
-        <v>353.30000000000007</v>
+        <v>5340.7000000000007</v>
       </c>
     </row>
     <row r="221" spans="10:11" x14ac:dyDescent="0.25">
@@ -4985,7 +4987,7 @@
         <v>21.2</v>
       </c>
       <c r="K221">
-        <v>355.6</v>
+        <v>5380.4</v>
       </c>
     </row>
     <row r="222" spans="10:11" x14ac:dyDescent="0.25">
@@ -4993,7 +4995,7 @@
         <v>21.3</v>
       </c>
       <c r="K222">
-        <v>357.90000000000003</v>
+        <v>5420.1</v>
       </c>
     </row>
     <row r="223" spans="10:11" x14ac:dyDescent="0.25">
@@ -5001,7 +5003,7 @@
         <v>21.4</v>
       </c>
       <c r="K223">
-        <v>360.2</v>
+        <v>5459.7999999999993</v>
       </c>
     </row>
     <row r="224" spans="10:11" x14ac:dyDescent="0.25">
@@ -5009,7 +5011,7 @@
         <v>21.5</v>
       </c>
       <c r="K224">
-        <v>362.5</v>
+        <v>5499.5</v>
       </c>
     </row>
     <row r="225" spans="10:11" x14ac:dyDescent="0.25">
@@ -5017,7 +5019,7 @@
         <v>21.6</v>
       </c>
       <c r="K225">
-        <v>364.80000000000007</v>
+        <v>5539.2000000000007</v>
       </c>
     </row>
     <row r="226" spans="10:11" x14ac:dyDescent="0.25">
@@ -5025,7 +5027,7 @@
         <v>21.7</v>
       </c>
       <c r="K226">
-        <v>367.1</v>
+        <v>5578.9</v>
       </c>
     </row>
     <row r="227" spans="10:11" x14ac:dyDescent="0.25">
@@ -5033,7 +5035,7 @@
         <v>21.8</v>
       </c>
       <c r="K227">
-        <v>369.40000000000003</v>
+        <v>5618.6</v>
       </c>
     </row>
     <row r="228" spans="10:11" x14ac:dyDescent="0.25">
@@ -5041,7 +5043,7 @@
         <v>21.9</v>
       </c>
       <c r="K228">
-        <v>371.7</v>
+        <v>5658.2999999999993</v>
       </c>
     </row>
     <row r="229" spans="10:11" x14ac:dyDescent="0.25">
@@ -5049,7 +5051,7 @@
         <v>22</v>
       </c>
       <c r="K229">
-        <v>374</v>
+        <v>5698</v>
       </c>
     </row>
   </sheetData>
@@ -5097,7 +5099,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>21-Aug-2024</v>
+        <v>22-Aug-2024</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -5393,7 +5395,7 @@
       </c>
       <c r="B3" s="2" t="str" cm="1">
         <f t="array" aca="1" ref="B3" ca="1">HD_Date</f>
-        <v>21-Aug-2024</v>
+        <v>22-Aug-2024</v>
       </c>
       <c r="C3" s="2"/>
     </row>

</xml_diff>

<commit_message>
I see the cubic interpolates poorly
</commit_message>
<xml_diff>
--- a/AlternativeLinearInterpolation.xlsx
+++ b/AlternativeLinearInterpolation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8AC396F-5DED-45DB-93CA-A4F415637DEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10090A16-D8C1-4148-B5EF-B09276B9B4A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -641,10 +641,10 @@
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FF99CCFF"/>
       <color rgb="FFCCFFCC"/>
       <color rgb="FFEBFFEB"/>
       <color rgb="FFFF9999"/>
-      <color rgb="FF99CCFF"/>
       <color rgb="FFEFFFEF"/>
     </mruColors>
   </colors>
@@ -1753,6 +1753,1037 @@
             </c:ext>
           </c:extLst>
         </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Report!$J$19:$J$165</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="147"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>6.5000000000000098</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>6.8000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>6.9000000000000101</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>7.0000000000000098</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>7.2000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>7.3000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>7.4000000000000101</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>7.5000000000000098</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>7.6000000000000103</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>7.7000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>7.8000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>7.9000000000000101</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>8.0000000000000107</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>8.1000000000000103</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>8.2000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>8.3000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>8.4000000000000092</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>8.5000000000000107</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>8.6000000000000103</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>8.7000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>8.8000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>8.9000000000000092</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>9.0000000000000107</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>9.1000000000000103</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>9.2000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>9.3000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>9.4000000000000092</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>9.5000000000000107</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>9.6000000000000103</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>9.7000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>9.8000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>9.9000000000000092</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>10.1</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>10.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>10.3</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>10.4</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>10.9</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>11.1</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>11.3</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>11.4</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>11.6</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>11.7</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>11.9</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>12.2</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>12.3</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>12.4</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>12.6</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>12.7</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>12.8</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>12.9</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>13.1</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>13.2</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>13.3</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>13.4</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>13.6</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>13.7</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>13.8</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>13.9</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>14.1</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>14.2</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>14.3</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>14.4</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>14.6</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>14.7</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>14.8</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>14.9</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>15.1</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>15.2</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>15.3</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>15.4</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>15.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Report!$I$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-907E-4FD8-B585-ADAD90F25C9E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Report!$J$19:$J$165</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="147"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1000000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.2000000000000002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.2999999999999998</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.4</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.5</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.6</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.8</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.9</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.1</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.4</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3.5</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.7</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3.8</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.2</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>4.3</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.4000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.7</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.8</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4.9000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.0999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>5.2</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>5.3</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>5.4</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5.6</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5.7</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>6.1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>6.2</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>6.3</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>6.4</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>6.5000000000000098</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>6.6</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>6.7</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>6.8000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>6.9000000000000101</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>7.0000000000000098</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>7.1</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>7.2000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>7.3000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>7.4000000000000101</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>7.5000000000000098</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>7.6000000000000103</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>7.7000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>7.8000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>7.9000000000000101</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>8.0000000000000107</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>8.1000000000000103</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>8.2000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>8.3000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>8.4000000000000092</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>8.5000000000000107</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>8.6000000000000103</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>8.7000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>8.8000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>8.9000000000000092</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>9.0000000000000107</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>9.1000000000000103</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>9.2000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>9.3000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>9.4000000000000092</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>9.5000000000000107</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>9.6000000000000103</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>9.7000000000000099</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>9.8000000000000096</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>9.9000000000000092</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>10.1</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>10.199999999999999</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>10.3</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>10.4</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>10.5</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>10.6</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>10.7</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>10.9</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>11.1</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>11.2</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>11.3</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>11.4</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>11.5</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>11.6</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>11.7</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>11.8</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>11.9</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>12.1</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>12.2</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>12.3</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>12.4</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>12.5</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>12.6</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>12.7</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>12.8</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>12.9</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>13.1</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>13.2</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>13.3</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>13.4</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>13.5</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>13.6</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>13.7</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>13.8</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>13.9</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>14.1</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>14.2</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>14.3</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>14.4</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>14.5</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>14.6</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>14.7</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>14.8</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>14.9</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>15.1</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>15.2</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>15.3</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>15.4</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>15.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Report!$J$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-907E-4FD8-B585-ADAD90F25C9E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Exact</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="99CCFF"/>
+              </a:solidFill>
+              <a:ln w="31750">
+                <a:solidFill>
+                  <a:schemeClr val="accent5">
+                    <a:alpha val="99000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Report!$I$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Report!$J$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-907E-4FD8-B585-ADAD90F25C9E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -1831,7 +2862,7 @@
         <c:axId val="2122341135"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="-100"/>
+          <c:min val="-1000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3126,7 +4157,7 @@
   <dimension ref="A1:L229"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -3187,7 +4218,11 @@
         <v>26</v>
       </c>
       <c r="I7" s="10">
-        <v>8.3000000000000007</v>
+        <v>-5</v>
+      </c>
+      <c r="J7">
+        <f>_nx^3</f>
+        <v>-125</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -3207,7 +4242,7 @@
       </c>
       <c r="J8" cm="1">
         <f t="array" ref="J8">TREND(F17:F18,E17:E18,_nx)</f>
-        <v>259.10000000000036</v>
+        <v>-5021</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -3223,11 +4258,11 @@
       </c>
       <c r="I9" t="b">
         <f>_nx&lt;_nmin</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" cm="1">
         <f t="array" ref="J9">TREND(F7:F8,E7:E8,_nx)</f>
-        <v>52.100000000000016</v>
+        <v>-41.000000000000007</v>
       </c>
       <c r="K9" s="11"/>
       <c r="L9" s="11"/>
@@ -3245,18 +4280,18 @@
       </c>
       <c r="I10" t="b">
         <f>IF(MEDIAN(_nmin,_nmax,_nx)=_nx,TRUE,FALSE)</f>
-        <v>1</v>
-      </c>
-      <c r="J10" s="9">
+        <v>0</v>
+      </c>
+      <c r="J10" s="9" t="e">
         <f>_xlfn.XMATCH(_nx,_nData,-1)</f>
-        <v>8</v>
-      </c>
-      <c r="K10" s="10" cm="1">
+        <v>#N/A</v>
+      </c>
+      <c r="K10" s="10" t="e" cm="1">
         <f t="array" ref="K10:L10">J10+{0,1}</f>
-        <v>8</v>
-      </c>
-      <c r="L10" s="10">
-        <v>9</v>
+        <v>#N/A</v>
+      </c>
+      <c r="L10" s="10" t="e">
+        <v>#N/A</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -3270,13 +4305,13 @@
       <c r="J11" t="s">
         <v>27</v>
       </c>
-      <c r="K11" cm="1">
+      <c r="K11" t="e" cm="1">
         <f t="array" ref="K11">INDEX(_nData,K10)</f>
-        <v>8</v>
-      </c>
-      <c r="L11" cm="1">
+        <v>#N/A</v>
+      </c>
+      <c r="L11" t="e" cm="1">
         <f t="array" ref="L11">INDEX(_nData,L10)</f>
-        <v>9</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -3290,13 +4325,13 @@
       <c r="J12" t="s">
         <v>28</v>
       </c>
-      <c r="K12" cm="1">
+      <c r="K12" t="e" cm="1">
         <f t="array" ref="K12">INDEX($F$7:$F$18,K10)</f>
-        <v>512</v>
-      </c>
-      <c r="L12" cm="1">
+        <v>#N/A</v>
+      </c>
+      <c r="L12" t="e" cm="1">
         <f t="array" ref="L12">INDEX($F$7:$F$18,L10)</f>
-        <v>729</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -3307,9 +4342,9 @@
         <f t="shared" si="0"/>
         <v>343</v>
       </c>
-      <c r="K13" cm="1">
+      <c r="K13" t="e" cm="1">
         <f t="array" ref="K13">TREND(K12:L12,K11:L11,_nx)</f>
-        <v>577.10000000000014</v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -3322,7 +4357,7 @@
       </c>
       <c r="I14" cm="1">
         <f t="array" ref="I14">_xlfn.SWITCH(TRUE,I8,J8,I9,J9,K13)</f>
-        <v>577.10000000000014</v>
+        <v>-41.000000000000007</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -3362,7 +4397,7 @@
       </c>
       <c r="K18">
         <f>I14</f>
-        <v>577.10000000000014</v>
+        <v>-41.000000000000007</v>
       </c>
     </row>
     <row r="19" spans="5:11" x14ac:dyDescent="0.25">
@@ -5056,7 +6091,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Done with play. Now code
</commit_message>
<xml_diff>
--- a/AlternativeLinearInterpolation.xlsx
+++ b/AlternativeLinearInterpolation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10090A16-D8C1-4148-B5EF-B09276B9B4A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D96078F-6046-4765-8F1C-16604AF776E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -726,10 +726,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Report!$J$19:$J$165</c:f>
+              <c:f>Report!$J$19:$J$181</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="147"/>
+                <c:ptCount val="163"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -1170,16 +1170,64 @@
                 </c:pt>
                 <c:pt idx="146">
                   <c:v>15.6</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>15.7</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>15.8</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>15.9</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>16.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>16.2</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>16.3</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>16.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>16.5</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>16.600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>16.7</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>16.8</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>16.899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>17.100000000000001</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>17.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Report!$K$19:$K$165</c:f>
+              <c:f>Report!$K$19:$K$181</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="147"/>
+                <c:ptCount val="163"/>
                 <c:pt idx="0">
                   <c:v>0.99999999999999911</c:v>
                 </c:pt>
@@ -1620,6 +1668,54 @@
                 </c:pt>
                 <c:pt idx="146">
                   <c:v>3157.2</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>3196.8999999999996</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>3236.6000000000004</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>3276.3</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>3316</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>3355.7000000000007</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>3395.3999999999996</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>3435.1000000000004</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>3474.7999999999993</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>3514.5</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>3554.2000000000007</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>3593.8999999999996</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>3633.6000000000004</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>3673.2999999999993</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>3713</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>3752.7000000000007</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>3792.3999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4156,8 +4252,8 @@
   </sheetPr>
   <dimension ref="A1:L229"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="E6" workbookViewId="0">
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>